<commit_message>
Add special token "Month in a year"
</commit_message>
<xml_diff>
--- a/textToOps/data/raw/units.xlsx
+++ b/textToOps/data/raw/units.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heejinchae/Documents/github/Text2GeoAn/textToOps/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E70AE0F-013C-0541-BD16-FBAD83C4E094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D648D001-C8F6-7143-AB6A-8CAD0A85201A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48000" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{28EAAB28-9B20-3D40-8466-CD2F64D1E5AF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{28EAAB28-9B20-3D40-8466-CD2F64D1E5AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1DBA88-94D6-0D4F-9D8A-F80A228464A5}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>